<commit_message>
print more stats to console
</commit_message>
<xml_diff>
--- a/source_data_files_ncomms/SourceDataFigure1B.xlsx
+++ b/source_data_files_ncomms/SourceDataFigure1B.xlsx
@@ -13,7 +13,1867 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="744">
+  <si>
+    <t>rt_sr</t>
+  </si>
+  <si>
+    <t>rt_all</t>
+  </si>
+  <si>
+    <t>pc_sr</t>
+  </si>
+  <si>
+    <t>pc_all</t>
+  </si>
+  <si>
+    <t>cond</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>rt_sr</t>
+  </si>
+  <si>
+    <t>rt_all</t>
+  </si>
+  <si>
+    <t>pc_sr</t>
+  </si>
+  <si>
+    <t>pc_all</t>
+  </si>
+  <si>
+    <t>cond</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>rt_sr</t>
+  </si>
+  <si>
+    <t>rt_all</t>
+  </si>
+  <si>
+    <t>pc_sr</t>
+  </si>
+  <si>
+    <t>pc_all</t>
+  </si>
+  <si>
+    <t>cond</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>rt_sr</t>
+  </si>
+  <si>
+    <t>rt_all</t>
+  </si>
+  <si>
+    <t>pc_sr</t>
+  </si>
+  <si>
+    <t>pc_all</t>
+  </si>
+  <si>
+    <t>cond</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>rt_sr</t>
+  </si>
+  <si>
+    <t>rt_all</t>
+  </si>
+  <si>
+    <t>pc_sr</t>
+  </si>
+  <si>
+    <t>pc_all</t>
+  </si>
+  <si>
+    <t>cond</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>primed</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
   <si>
     <t>rt_sr</t>
   </si>
@@ -443,22 +2303,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>620</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1</v>
+        <v>621</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>2</v>
+        <v>622</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>3</v>
+        <v>623</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>4</v>
+        <v>624</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>123</v>
+        <v>743</v>
       </c>
     </row>
     <row r="2">
@@ -475,7 +2335,7 @@
         <v>99.600000000000009</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>5</v>
+        <v>625</v>
       </c>
       <c r="F2" s="0">
         <v>30</v>
@@ -495,7 +2355,7 @@
         <v>96</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>6</v>
+        <v>626</v>
       </c>
       <c r="F3" s="0">
         <v>30</v>
@@ -515,7 +2375,7 @@
         <v>99.200000000000003</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>7</v>
+        <v>627</v>
       </c>
       <c r="F4" s="0">
         <v>30</v>
@@ -535,7 +2395,7 @@
         <v>98</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>8</v>
+        <v>628</v>
       </c>
       <c r="F5" s="0">
         <v>30</v>
@@ -555,7 +2415,7 @@
         <v>99.600000000000009</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>9</v>
+        <v>629</v>
       </c>
       <c r="F6" s="0">
         <v>30</v>
@@ -575,7 +2435,7 @@
         <v>99</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>10</v>
+        <v>630</v>
       </c>
       <c r="F7" s="0">
         <v>30</v>
@@ -595,7 +2455,7 @@
         <v>99.799999999999997</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>11</v>
+        <v>631</v>
       </c>
       <c r="F8" s="0">
         <v>31</v>
@@ -615,7 +2475,7 @@
         <v>98</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>12</v>
+        <v>632</v>
       </c>
       <c r="F9" s="0">
         <v>31</v>
@@ -635,7 +2495,7 @@
         <v>99.799999999999997</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>13</v>
+        <v>633</v>
       </c>
       <c r="F10" s="0">
         <v>31</v>
@@ -655,7 +2515,7 @@
         <v>95</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>14</v>
+        <v>634</v>
       </c>
       <c r="F11" s="0">
         <v>31</v>
@@ -675,7 +2535,7 @@
         <v>99.600000000000009</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>15</v>
+        <v>635</v>
       </c>
       <c r="F12" s="0">
         <v>31</v>
@@ -695,7 +2555,7 @@
         <v>98</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>16</v>
+        <v>636</v>
       </c>
       <c r="F13" s="0">
         <v>31</v>
@@ -715,7 +2575,7 @@
         <v>100</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>17</v>
+        <v>637</v>
       </c>
       <c r="F14" s="0">
         <v>32</v>
@@ -735,7 +2595,7 @@
         <v>100</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>18</v>
+        <v>638</v>
       </c>
       <c r="F15" s="0">
         <v>32</v>
@@ -755,7 +2615,7 @@
         <v>100</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>19</v>
+        <v>639</v>
       </c>
       <c r="F16" s="0">
         <v>32</v>
@@ -775,7 +2635,7 @@
         <v>100</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>20</v>
+        <v>640</v>
       </c>
       <c r="F17" s="0">
         <v>32</v>
@@ -795,7 +2655,7 @@
         <v>100</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>21</v>
+        <v>641</v>
       </c>
       <c r="F18" s="0">
         <v>32</v>
@@ -815,7 +2675,7 @@
         <v>98</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>22</v>
+        <v>642</v>
       </c>
       <c r="F19" s="0">
         <v>32</v>
@@ -835,7 +2695,7 @@
         <v>99.799999999999997</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>23</v>
+        <v>643</v>
       </c>
       <c r="F20" s="0">
         <v>32</v>
@@ -855,7 +2715,7 @@
         <v>98</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>24</v>
+        <v>644</v>
       </c>
       <c r="F21" s="0">
         <v>32</v>
@@ -875,7 +2735,7 @@
         <v>99.200000000000003</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>25</v>
+        <v>645</v>
       </c>
       <c r="F22" s="0">
         <v>32</v>
@@ -895,7 +2755,7 @@
         <v>96</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>26</v>
+        <v>646</v>
       </c>
       <c r="F23" s="0">
         <v>32</v>
@@ -915,7 +2775,7 @@
         <v>99</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>27</v>
+        <v>647</v>
       </c>
       <c r="F24" s="0">
         <v>32</v>
@@ -935,7 +2795,7 @@
         <v>98</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>28</v>
+        <v>648</v>
       </c>
       <c r="F25" s="0">
         <v>32</v>
@@ -955,7 +2815,7 @@
         <v>99.400000000000006</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>29</v>
+        <v>649</v>
       </c>
       <c r="F26" s="0">
         <v>33</v>
@@ -975,7 +2835,7 @@
         <v>98</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>30</v>
+        <v>650</v>
       </c>
       <c r="F27" s="0">
         <v>33</v>
@@ -995,7 +2855,7 @@
         <v>99.200000000000003</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>31</v>
+        <v>651</v>
       </c>
       <c r="F28" s="0">
         <v>33</v>
@@ -1015,7 +2875,7 @@
         <v>96</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>32</v>
+        <v>652</v>
       </c>
       <c r="F29" s="0">
         <v>33</v>
@@ -1035,7 +2895,7 @@
         <v>99.799999999999997</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>33</v>
+        <v>653</v>
       </c>
       <c r="F30" s="0">
         <v>34</v>
@@ -1055,7 +2915,7 @@
         <v>98</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>34</v>
+        <v>654</v>
       </c>
       <c r="F31" s="0">
         <v>34</v>
@@ -1075,7 +2935,7 @@
         <v>99.400000000000006</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>35</v>
+        <v>655</v>
       </c>
       <c r="F32" s="0">
         <v>34</v>
@@ -1095,7 +2955,7 @@
         <v>93</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>36</v>
+        <v>656</v>
       </c>
       <c r="F33" s="0">
         <v>34</v>
@@ -1115,7 +2975,7 @@
         <v>99.200000000000003</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>37</v>
+        <v>657</v>
       </c>
       <c r="F34" s="0">
         <v>34</v>
@@ -1135,7 +2995,7 @@
         <v>87</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>38</v>
+        <v>658</v>
       </c>
       <c r="F35" s="0">
         <v>34</v>
@@ -1155,7 +3015,7 @@
         <v>99.799999999999997</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>39</v>
+        <v>659</v>
       </c>
       <c r="F36" s="0">
         <v>34</v>
@@ -1175,7 +3035,7 @@
         <v>98</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>40</v>
+        <v>660</v>
       </c>
       <c r="F37" s="0">
         <v>34</v>
@@ -1195,7 +3055,7 @@
         <v>99.600000000000009</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>41</v>
+        <v>661</v>
       </c>
       <c r="F38" s="0">
         <v>34</v>
@@ -1215,7 +3075,7 @@
         <v>98</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>42</v>
+        <v>662</v>
       </c>
       <c r="F39" s="0">
         <v>34</v>
@@ -1235,7 +3095,7 @@
         <v>98.200000000000003</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>43</v>
+        <v>663</v>
       </c>
       <c r="F40" s="0">
         <v>35</v>
@@ -1255,7 +3115,7 @@
         <v>94</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>44</v>
+        <v>664</v>
       </c>
       <c r="F41" s="0">
         <v>35</v>
@@ -1275,7 +3135,7 @@
         <v>99.400000000000006</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>45</v>
+        <v>665</v>
       </c>
       <c r="F42" s="0">
         <v>35</v>
@@ -1295,7 +3155,7 @@
         <v>96</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>46</v>
+        <v>666</v>
       </c>
       <c r="F43" s="0">
         <v>35</v>
@@ -1315,7 +3175,7 @@
         <v>99.200000000000003</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>47</v>
+        <v>667</v>
       </c>
       <c r="F44" s="0">
         <v>37</v>
@@ -1335,7 +3195,7 @@
         <v>100</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>48</v>
+        <v>668</v>
       </c>
       <c r="F45" s="0">
         <v>37</v>
@@ -1355,7 +3215,7 @@
         <v>98.200000000000003</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>49</v>
+        <v>669</v>
       </c>
       <c r="F46" s="0">
         <v>37</v>
@@ -1375,7 +3235,7 @@
         <v>93</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>50</v>
+        <v>670</v>
       </c>
       <c r="F47" s="0">
         <v>37</v>
@@ -1395,7 +3255,7 @@
         <v>96.400000000000006</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>51</v>
+        <v>671</v>
       </c>
       <c r="F48" s="0">
         <v>37</v>
@@ -1415,7 +3275,7 @@
         <v>90</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>52</v>
+        <v>672</v>
       </c>
       <c r="F49" s="0">
         <v>37</v>
@@ -1435,7 +3295,7 @@
         <v>98.799999999999983</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>53</v>
+        <v>673</v>
       </c>
       <c r="F50" s="0">
         <v>37</v>
@@ -1455,7 +3315,7 @@
         <v>96</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>54</v>
+        <v>674</v>
       </c>
       <c r="F51" s="0">
         <v>37</v>
@@ -1475,7 +3335,7 @@
         <v>99.400000000000006</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>55</v>
+        <v>675</v>
       </c>
       <c r="F52" s="0">
         <v>39</v>
@@ -1495,7 +3355,7 @@
         <v>99</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>56</v>
+        <v>676</v>
       </c>
       <c r="F53" s="0">
         <v>39</v>
@@ -1515,7 +3375,7 @@
         <v>99.600000000000009</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>57</v>
+        <v>677</v>
       </c>
       <c r="F54" s="0">
         <v>39</v>
@@ -1535,7 +3395,7 @@
         <v>100</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>58</v>
+        <v>678</v>
       </c>
       <c r="F55" s="0">
         <v>39</v>
@@ -1555,7 +3415,7 @@
         <v>100</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>59</v>
+        <v>679</v>
       </c>
       <c r="F56" s="0">
         <v>40</v>
@@ -1575,7 +3435,7 @@
         <v>98</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>60</v>
+        <v>680</v>
       </c>
       <c r="F57" s="0">
         <v>40</v>
@@ -1595,7 +3455,7 @@
         <v>99.400000000000006</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>61</v>
+        <v>681</v>
       </c>
       <c r="F58" s="0">
         <v>41</v>
@@ -1615,7 +3475,7 @@
         <v>94</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>62</v>
+        <v>682</v>
       </c>
       <c r="F59" s="0">
         <v>41</v>
@@ -1635,7 +3495,7 @@
         <v>97.799999999999997</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>63</v>
+        <v>683</v>
       </c>
       <c r="F60" s="0">
         <v>41</v>
@@ -1655,7 +3515,7 @@
         <v>94</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>64</v>
+        <v>684</v>
       </c>
       <c r="F61" s="0">
         <v>41</v>
@@ -1675,7 +3535,7 @@
         <v>100</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>65</v>
+        <v>685</v>
       </c>
       <c r="F62" s="0">
         <v>42</v>
@@ -1695,7 +3555,7 @@
         <v>100</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>66</v>
+        <v>686</v>
       </c>
       <c r="F63" s="0">
         <v>42</v>
@@ -1715,7 +3575,7 @@
         <v>99.799999999999997</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>67</v>
+        <v>687</v>
       </c>
       <c r="F64" s="0">
         <v>42</v>
@@ -1735,7 +3595,7 @@
         <v>98</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>68</v>
+        <v>688</v>
       </c>
       <c r="F65" s="0">
         <v>42</v>
@@ -1755,7 +3615,7 @@
         <v>100</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>69</v>
+        <v>689</v>
       </c>
       <c r="F66" s="0">
         <v>42</v>
@@ -1775,7 +3635,7 @@
         <v>99</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>70</v>
+        <v>690</v>
       </c>
       <c r="F67" s="0">
         <v>42</v>
@@ -1795,7 +3655,7 @@
         <v>92.799999999999997</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>71</v>
+        <v>691</v>
       </c>
       <c r="F68" s="0">
         <v>43</v>
@@ -1815,7 +3675,7 @@
         <v>94</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>72</v>
+        <v>692</v>
       </c>
       <c r="F69" s="0">
         <v>43</v>
@@ -1835,7 +3695,7 @@
         <v>90</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>73</v>
+        <v>693</v>
       </c>
       <c r="F70" s="0">
         <v>43</v>
@@ -1855,7 +3715,7 @@
         <v>95</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>74</v>
+        <v>694</v>
       </c>
       <c r="F71" s="0">
         <v>43</v>
@@ -1875,7 +3735,7 @@
         <v>98.599999999999994</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>75</v>
+        <v>695</v>
       </c>
       <c r="F72" s="0">
         <v>44</v>
@@ -1895,7 +3755,7 @@
         <v>92</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>76</v>
+        <v>696</v>
       </c>
       <c r="F73" s="0">
         <v>44</v>
@@ -1915,7 +3775,7 @@
         <v>99.799999999999997</v>
       </c>
       <c r="E74" s="0" t="s">
-        <v>77</v>
+        <v>697</v>
       </c>
       <c r="F74" s="0">
         <v>44</v>
@@ -1935,7 +3795,7 @@
         <v>96</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>78</v>
+        <v>698</v>
       </c>
       <c r="F75" s="0">
         <v>44</v>
@@ -1955,7 +3815,7 @@
         <v>99.799999999999997</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>79</v>
+        <v>699</v>
       </c>
       <c r="F76" s="0">
         <v>44</v>
@@ -1975,7 +3835,7 @@
         <v>96</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>80</v>
+        <v>700</v>
       </c>
       <c r="F77" s="0">
         <v>44</v>
@@ -1995,7 +3855,7 @@
         <v>99.799999999999997</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>81</v>
+        <v>701</v>
       </c>
       <c r="F78" s="0">
         <v>44</v>
@@ -2015,7 +3875,7 @@
         <v>97</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>82</v>
+        <v>702</v>
       </c>
       <c r="F79" s="0">
         <v>44</v>
@@ -2035,7 +3895,7 @@
         <v>98.200000000000003</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>83</v>
+        <v>703</v>
       </c>
       <c r="F80" s="0">
         <v>45</v>
@@ -2055,7 +3915,7 @@
         <v>97</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>84</v>
+        <v>704</v>
       </c>
       <c r="F81" s="0">
         <v>45</v>
@@ -2075,7 +3935,7 @@
         <v>97.399999999999991</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>85</v>
+        <v>705</v>
       </c>
       <c r="F82" s="0">
         <v>46</v>
@@ -2095,7 +3955,7 @@
         <v>97</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>86</v>
+        <v>706</v>
       </c>
       <c r="F83" s="0">
         <v>46</v>
@@ -2115,7 +3975,7 @@
         <v>97.800000000000011</v>
       </c>
       <c r="E84" s="0" t="s">
-        <v>87</v>
+        <v>707</v>
       </c>
       <c r="F84" s="0">
         <v>46</v>
@@ -2135,7 +3995,7 @@
         <v>98</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>88</v>
+        <v>708</v>
       </c>
       <c r="F85" s="0">
         <v>46</v>
@@ -2155,7 +4015,7 @@
         <v>91.000000000000014</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>89</v>
+        <v>709</v>
       </c>
       <c r="F86" s="0">
         <v>47</v>
@@ -2175,7 +4035,7 @@
         <v>87</v>
       </c>
       <c r="E87" s="0" t="s">
-        <v>90</v>
+        <v>710</v>
       </c>
       <c r="F87" s="0">
         <v>47</v>
@@ -2195,7 +4055,7 @@
         <v>99.200000000000003</v>
       </c>
       <c r="E88" s="0" t="s">
-        <v>91</v>
+        <v>711</v>
       </c>
       <c r="F88" s="0">
         <v>48</v>
@@ -2215,7 +4075,7 @@
         <v>100</v>
       </c>
       <c r="E89" s="0" t="s">
-        <v>92</v>
+        <v>712</v>
       </c>
       <c r="F89" s="0">
         <v>48</v>
@@ -2235,7 +4095,7 @@
         <v>100</v>
       </c>
       <c r="E90" s="0" t="s">
-        <v>93</v>
+        <v>713</v>
       </c>
       <c r="F90" s="0">
         <v>48</v>
@@ -2255,7 +4115,7 @@
         <v>100</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>94</v>
+        <v>714</v>
       </c>
       <c r="F91" s="0">
         <v>48</v>
@@ -2275,7 +4135,7 @@
         <v>92</v>
       </c>
       <c r="E92" s="0" t="s">
-        <v>95</v>
+        <v>715</v>
       </c>
       <c r="F92" s="0">
         <v>49</v>
@@ -2295,7 +4155,7 @@
         <v>96</v>
       </c>
       <c r="E93" s="0" t="s">
-        <v>96</v>
+        <v>716</v>
       </c>
       <c r="F93" s="0">
         <v>49</v>
@@ -2315,7 +4175,7 @@
         <v>100</v>
       </c>
       <c r="E94" s="0" t="s">
-        <v>97</v>
+        <v>717</v>
       </c>
       <c r="F94" s="0">
         <v>49</v>
@@ -2335,7 +4195,7 @@
         <v>98</v>
       </c>
       <c r="E95" s="0" t="s">
-        <v>98</v>
+        <v>718</v>
       </c>
       <c r="F95" s="0">
         <v>49</v>
@@ -2355,7 +4215,7 @@
         <v>97.800000000000011</v>
       </c>
       <c r="E96" s="0" t="s">
-        <v>99</v>
+        <v>719</v>
       </c>
       <c r="F96" s="0">
         <v>50</v>
@@ -2375,7 +4235,7 @@
         <v>96</v>
       </c>
       <c r="E97" s="0" t="s">
-        <v>100</v>
+        <v>720</v>
       </c>
       <c r="F97" s="0">
         <v>50</v>
@@ -2395,7 +4255,7 @@
         <v>99.200000000000003</v>
       </c>
       <c r="E98" s="0" t="s">
-        <v>101</v>
+        <v>721</v>
       </c>
       <c r="F98" s="0">
         <v>50</v>
@@ -2415,7 +4275,7 @@
         <v>97</v>
       </c>
       <c r="E99" s="0" t="s">
-        <v>102</v>
+        <v>722</v>
       </c>
       <c r="F99" s="0">
         <v>50</v>
@@ -2435,7 +4295,7 @@
         <v>100</v>
       </c>
       <c r="E100" s="0" t="s">
-        <v>103</v>
+        <v>723</v>
       </c>
       <c r="F100" s="0">
         <v>50</v>
@@ -2455,7 +4315,7 @@
         <v>99</v>
       </c>
       <c r="E101" s="0" t="s">
-        <v>104</v>
+        <v>724</v>
       </c>
       <c r="F101" s="0">
         <v>50</v>
@@ -2475,7 +4335,7 @@
         <v>97</v>
       </c>
       <c r="E102" s="0" t="s">
-        <v>105</v>
+        <v>725</v>
       </c>
       <c r="F102" s="0">
         <v>52</v>
@@ -2495,7 +4355,7 @@
         <v>98</v>
       </c>
       <c r="E103" s="0" t="s">
-        <v>106</v>
+        <v>726</v>
       </c>
       <c r="F103" s="0">
         <v>52</v>
@@ -2515,7 +4375,7 @@
         <v>99.799999999999997</v>
       </c>
       <c r="E104" s="0" t="s">
-        <v>107</v>
+        <v>727</v>
       </c>
       <c r="F104" s="0">
         <v>52</v>
@@ -2535,7 +4395,7 @@
         <v>98</v>
       </c>
       <c r="E105" s="0" t="s">
-        <v>108</v>
+        <v>728</v>
       </c>
       <c r="F105" s="0">
         <v>52</v>
@@ -2555,7 +4415,7 @@
         <v>99.600000000000009</v>
       </c>
       <c r="E106" s="0" t="s">
-        <v>109</v>
+        <v>729</v>
       </c>
       <c r="F106" s="0">
         <v>53</v>
@@ -2575,7 +4435,7 @@
         <v>100</v>
       </c>
       <c r="E107" s="0" t="s">
-        <v>110</v>
+        <v>730</v>
       </c>
       <c r="F107" s="0">
         <v>53</v>
@@ -2595,7 +4455,7 @@
         <v>100</v>
       </c>
       <c r="E108" s="0" t="s">
-        <v>111</v>
+        <v>731</v>
       </c>
       <c r="F108" s="0">
         <v>53</v>
@@ -2615,7 +4475,7 @@
         <v>100</v>
       </c>
       <c r="E109" s="0" t="s">
-        <v>112</v>
+        <v>732</v>
       </c>
       <c r="F109" s="0">
         <v>53</v>
@@ -2635,7 +4495,7 @@
         <v>98.800000000000011</v>
       </c>
       <c r="E110" s="0" t="s">
-        <v>113</v>
+        <v>733</v>
       </c>
       <c r="F110" s="0">
         <v>54</v>
@@ -2655,7 +4515,7 @@
         <v>94</v>
       </c>
       <c r="E111" s="0" t="s">
-        <v>114</v>
+        <v>734</v>
       </c>
       <c r="F111" s="0">
         <v>54</v>
@@ -2675,7 +4535,7 @@
         <v>96.799999999999997</v>
       </c>
       <c r="E112" s="0" t="s">
-        <v>115</v>
+        <v>735</v>
       </c>
       <c r="F112" s="0">
         <v>56</v>
@@ -2695,7 +4555,7 @@
         <v>99</v>
       </c>
       <c r="E113" s="0" t="s">
-        <v>116</v>
+        <v>736</v>
       </c>
       <c r="F113" s="0">
         <v>56</v>
@@ -2715,7 +4575,7 @@
         <v>100</v>
       </c>
       <c r="E114" s="0" t="s">
-        <v>117</v>
+        <v>737</v>
       </c>
       <c r="F114" s="0">
         <v>56</v>
@@ -2735,7 +4595,7 @@
         <v>100</v>
       </c>
       <c r="E115" s="0" t="s">
-        <v>118</v>
+        <v>738</v>
       </c>
       <c r="F115" s="0">
         <v>56</v>
@@ -2755,7 +4615,7 @@
         <v>99.799999999999997</v>
       </c>
       <c r="E116" s="0" t="s">
-        <v>119</v>
+        <v>739</v>
       </c>
       <c r="F116" s="0">
         <v>57</v>
@@ -2775,7 +4635,7 @@
         <v>97</v>
       </c>
       <c r="E117" s="0" t="s">
-        <v>120</v>
+        <v>740</v>
       </c>
       <c r="F117" s="0">
         <v>57</v>
@@ -2795,7 +4655,7 @@
         <v>100</v>
       </c>
       <c r="E118" s="0" t="s">
-        <v>121</v>
+        <v>741</v>
       </c>
       <c r="F118" s="0">
         <v>59</v>
@@ -2815,7 +4675,7 @@
         <v>99</v>
       </c>
       <c r="E119" s="0" t="s">
-        <v>122</v>
+        <v>742</v>
       </c>
       <c r="F119" s="0">
         <v>59</v>

</xml_diff>